<commit_message>
Tweak SOT package and fix typo in Excel data
git-svn-id: svn+ssh://bbfs-01.calit2.net/grw/Gordon/svn/trunk/Gadgets/Libraries/Parts@21486 2cf53259-273a-af40-bda6-69d31023b8ec
</commit_message>
<xml_diff>
--- a/Digikey/PN-Mosfets.xlsx
+++ b/Digikey/PN-Mosfets.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28725" windowHeight="10800" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28725" windowHeight="10800"/>
   </bookViews>
   <sheets>
     <sheet name="N-MOSFETS-SMD" sheetId="5" r:id="rId1"/>
@@ -3218,11 +3218,15 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="AC24" sqref="AC24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="25.42578125" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -5159,7 +5163,7 @@
         <v>204</v>
       </c>
       <c r="AC24" s="1" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
     </row>
     <row r="25" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -6291,6 +6295,7 @@
     <hyperlink ref="A29" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -10370,7 +10375,7 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Cleanup before merge with Koala - more needed than expected
git-svn-id: svn+ssh://bbfs-01.calit2.net/grw/Gordon/svn/trunk/Gadgets/Libraries/Parts@21489 2cf53259-273a-af40-bda6-69d31023b8ec
</commit_message>
<xml_diff>
--- a/Digikey/PN-Mosfets.xlsx
+++ b/Digikey/PN-Mosfets.xlsx
@@ -5,11 +5,11 @@
   <workbookPr dateCompatibility="0" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephen Deiss\Documents\eagle\Extra_Eagle_Libs\DigiKey\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\PCB Libraries\Library Expert 2015\Libraries\NVSL-Footprint-Library\Eagle\DigiKey\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28725" windowHeight="10800"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28725" windowHeight="10800" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="N-MOSFETS-SMD" sheetId="5" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="2058" uniqueCount="786">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="2059" uniqueCount="787">
   <si>
     <t>Datasheets</t>
   </si>
@@ -2372,9 +2372,6 @@
     <t>SOTFL50P160X60-6_HS</t>
   </si>
   <si>
-    <t>TO_92-3_Universal_HS</t>
-  </si>
-  <si>
     <t>TO456P990X238-3_HS</t>
   </si>
   <si>
@@ -2385,6 +2382,12 @@
   </si>
   <si>
     <t>I-PAK_TO-251AA_HS</t>
+  </si>
+  <si>
+    <t>TO254P1524X1054X470-3</t>
+  </si>
+  <si>
+    <t>TO-92-3_HS</t>
   </si>
 </sst>
 </file>
@@ -3218,14 +3221,15 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="AC24" sqref="AC24"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="25.42578125" customWidth="1"/>
     <col min="4" max="4" width="21.28515625" customWidth="1"/>
+    <col min="24" max="24" width="25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -5000,7 +5004,7 @@
         <v>315</v>
       </c>
       <c r="AC22" s="1" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="23" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -5083,7 +5087,7 @@
         <v>767</v>
       </c>
       <c r="AC23" s="1" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="24" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -5326,7 +5330,7 @@
         <v>428</v>
       </c>
       <c r="AC26" s="1" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
     </row>
     <row r="27" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -5726,7 +5730,7 @@
         <v>481</v>
       </c>
       <c r="AC31" s="1" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="32" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -6303,8 +6307,8 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="AC6" sqref="AC6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6475,7 +6479,7 @@
         <v>306</v>
       </c>
       <c r="AC2" s="1" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="3" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -6558,7 +6562,7 @@
         <v>767</v>
       </c>
       <c r="AC3" s="1" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="4" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -6638,7 +6642,7 @@
         <v>328</v>
       </c>
       <c r="AC4" s="1" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="5" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -6721,7 +6725,7 @@
         <v>767</v>
       </c>
       <c r="AC5" s="1" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="6" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -6801,7 +6805,7 @@
         <v>639</v>
       </c>
       <c r="AC6" s="1" t="s">
-        <v>781</v>
+        <v>786</v>
       </c>
     </row>
     <row r="7" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -6881,7 +6885,7 @@
         <v>639</v>
       </c>
       <c r="AC7" s="1" t="s">
-        <v>781</v>
+        <v>786</v>
       </c>
     </row>
     <row r="8" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -6961,7 +6965,7 @@
         <v>639</v>
       </c>
       <c r="AC8" s="1" t="s">
-        <v>781</v>
+        <v>786</v>
       </c>
     </row>
     <row r="9" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -7041,7 +7045,7 @@
         <v>639</v>
       </c>
       <c r="AC9" s="1" t="s">
-        <v>781</v>
+        <v>786</v>
       </c>
     </row>
     <row r="10" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -7121,7 +7125,7 @@
         <v>639</v>
       </c>
       <c r="AC10" s="1" t="s">
-        <v>781</v>
+        <v>786</v>
       </c>
     </row>
     <row r="11" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -7201,7 +7205,7 @@
         <v>639</v>
       </c>
       <c r="AC11" s="1" t="s">
-        <v>781</v>
+        <v>786</v>
       </c>
     </row>
     <row r="12" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -7281,7 +7285,7 @@
         <v>639</v>
       </c>
       <c r="AC12" s="1" t="s">
-        <v>781</v>
+        <v>786</v>
       </c>
     </row>
     <row r="13" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -7361,7 +7365,7 @@
         <v>639</v>
       </c>
       <c r="AC13" s="1" t="s">
-        <v>781</v>
+        <v>786</v>
       </c>
     </row>
     <row r="14" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -7441,7 +7445,7 @@
         <v>639</v>
       </c>
       <c r="AC14" s="1" t="s">
-        <v>781</v>
+        <v>786</v>
       </c>
     </row>
     <row r="15" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -7521,7 +7525,7 @@
         <v>639</v>
       </c>
       <c r="AC15" s="1" t="s">
-        <v>781</v>
+        <v>786</v>
       </c>
     </row>
     <row r="16" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -7601,7 +7605,7 @@
         <v>639</v>
       </c>
       <c r="AC16" s="1" t="s">
-        <v>781</v>
+        <v>786</v>
       </c>
     </row>
     <row r="17" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -7681,7 +7685,7 @@
         <v>639</v>
       </c>
       <c r="AC17" s="1" t="s">
-        <v>781</v>
+        <v>786</v>
       </c>
     </row>
     <row r="18" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -7761,7 +7765,7 @@
         <v>639</v>
       </c>
       <c r="AC18" s="1" t="s">
-        <v>781</v>
+        <v>786</v>
       </c>
     </row>
     <row r="19" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -7841,7 +7845,7 @@
         <v>639</v>
       </c>
       <c r="AC19" s="1" t="s">
-        <v>781</v>
+        <v>786</v>
       </c>
     </row>
     <row r="20" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -7921,7 +7925,7 @@
         <v>639</v>
       </c>
       <c r="AC20" s="1" t="s">
-        <v>781</v>
+        <v>786</v>
       </c>
     </row>
   </sheetData>
@@ -7929,6 +7933,7 @@
     <hyperlink ref="A3" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -7936,11 +7941,15 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.5703125" customWidth="1"/>
+    <col min="24" max="24" width="33.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -9877,7 +9886,7 @@
         <v>580</v>
       </c>
       <c r="AC24" s="1" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="25" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -10368,6 +10377,7 @@
     <hyperlink ref="A18" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -10375,8 +10385,8 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H39" sqref="H39"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Y2" sqref="Y2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10549,6 +10559,9 @@
       <c r="AA2" s="1" t="s">
         <v>767</v>
       </c>
+      <c r="AC2" s="1" t="s">
+        <v>785</v>
+      </c>
     </row>
     <row r="3" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -10627,7 +10640,7 @@
         <v>639</v>
       </c>
       <c r="AC3" s="1" t="s">
-        <v>781</v>
+        <v>786</v>
       </c>
     </row>
     <row r="4" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -10707,7 +10720,7 @@
         <v>639</v>
       </c>
       <c r="AC4" s="1" t="s">
-        <v>781</v>
+        <v>786</v>
       </c>
     </row>
     <row r="5" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -10787,7 +10800,7 @@
         <v>639</v>
       </c>
       <c r="AC5" s="1" t="s">
-        <v>781</v>
+        <v>786</v>
       </c>
     </row>
     <row r="6" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -10867,7 +10880,7 @@
         <v>639</v>
       </c>
       <c r="AC6" s="1" t="s">
-        <v>781</v>
+        <v>786</v>
       </c>
     </row>
     <row r="7" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -10947,7 +10960,7 @@
         <v>639</v>
       </c>
       <c r="AC7" s="1" t="s">
-        <v>781</v>
+        <v>786</v>
       </c>
     </row>
     <row r="8" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -11027,10 +11040,11 @@
         <v>639</v>
       </c>
       <c r="AC8" s="1" t="s">
-        <v>781</v>
+        <v>786</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>